<commit_message>
success: first global map
map visualization to be fixed , testing with 0 cost of moving
</commit_message>
<xml_diff>
--- a/Data/Global Data/Population_Country.xlsx
+++ b/Data/Global Data/Population_Country.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\18-6 Data\structural_zeros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balbi\git\migration\Data\Global Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
-    <sheet name="18_0s" sheetId="1" r:id="rId1"/>
+    <sheet name="population" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1625,8 +1625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Adjusted variable names in datasets
adjusted variable names in population and SDG datasets to be compatible (var names can't be numbers)
</commit_message>
<xml_diff>
--- a/Data/Global Data/Population_Country.xlsx
+++ b/Data/Global Data/Population_Country.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balbi\git\migration\Data\Global Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ab6176\Documents\GitHub\migration\Data\Global Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9375"/>
   </bookViews>
   <sheets>
     <sheet name="population" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="293">
   <si>
     <t>Country</t>
   </si>
@@ -814,12 +814,96 @@
   </si>
   <si>
     <t>'Paracel Islands'</t>
+  </si>
+  <si>
+    <t>x1990</t>
+  </si>
+  <si>
+    <t>x1991</t>
+  </si>
+  <si>
+    <t>x1992</t>
+  </si>
+  <si>
+    <t>x1993</t>
+  </si>
+  <si>
+    <t>x1994</t>
+  </si>
+  <si>
+    <t>x1995</t>
+  </si>
+  <si>
+    <t>x1996</t>
+  </si>
+  <si>
+    <t>x1997</t>
+  </si>
+  <si>
+    <t>x1998</t>
+  </si>
+  <si>
+    <t>x1999</t>
+  </si>
+  <si>
+    <t>x2000</t>
+  </si>
+  <si>
+    <t>x2001</t>
+  </si>
+  <si>
+    <t>x2002</t>
+  </si>
+  <si>
+    <t>x2003</t>
+  </si>
+  <si>
+    <t>x2004</t>
+  </si>
+  <si>
+    <t>x2005</t>
+  </si>
+  <si>
+    <t>x2006</t>
+  </si>
+  <si>
+    <t>x2007</t>
+  </si>
+  <si>
+    <t>x2008</t>
+  </si>
+  <si>
+    <t>x2009</t>
+  </si>
+  <si>
+    <t>x2010</t>
+  </si>
+  <si>
+    <t>x2011</t>
+  </si>
+  <si>
+    <t>x2012</t>
+  </si>
+  <si>
+    <t>x2013</t>
+  </si>
+  <si>
+    <t>x2014</t>
+  </si>
+  <si>
+    <t>x2015</t>
+  </si>
+  <si>
+    <t>x2016</t>
+  </si>
+  <si>
+    <t>x2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1622,105 +1706,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD265"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AB7" sqref="AB7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
-        <v>1990</v>
-      </c>
-      <c r="D1">
-        <v>1991</v>
-      </c>
-      <c r="E1">
-        <v>1992</v>
-      </c>
-      <c r="F1">
-        <v>1993</v>
-      </c>
-      <c r="G1">
-        <v>1994</v>
-      </c>
-      <c r="H1">
-        <v>1995</v>
-      </c>
-      <c r="I1">
-        <v>1996</v>
-      </c>
-      <c r="J1">
-        <v>1997</v>
-      </c>
-      <c r="K1">
-        <v>1998</v>
-      </c>
-      <c r="L1">
-        <v>1999</v>
-      </c>
-      <c r="M1">
-        <v>2000</v>
-      </c>
-      <c r="N1">
-        <v>2001</v>
-      </c>
-      <c r="O1">
-        <v>2002</v>
-      </c>
-      <c r="P1">
-        <v>2003</v>
-      </c>
-      <c r="Q1">
-        <v>2004</v>
-      </c>
-      <c r="R1">
-        <v>2005</v>
-      </c>
-      <c r="S1">
-        <v>2006</v>
-      </c>
-      <c r="T1">
-        <v>2007</v>
-      </c>
-      <c r="U1">
-        <v>2008</v>
-      </c>
-      <c r="V1">
-        <v>2009</v>
-      </c>
-      <c r="W1">
-        <v>2010</v>
-      </c>
-      <c r="X1">
-        <v>2011</v>
-      </c>
-      <c r="Y1">
-        <v>2012</v>
-      </c>
-      <c r="Z1">
-        <v>2013</v>
-      </c>
-      <c r="AA1">
-        <v>2014</v>
-      </c>
-      <c r="AB1">
-        <v>2015</v>
-      </c>
-      <c r="AC1">
-        <v>2016</v>
-      </c>
-      <c r="AD1">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G1" t="s">
+        <v>269</v>
+      </c>
+      <c r="H1" t="s">
+        <v>270</v>
+      </c>
+      <c r="I1" t="s">
+        <v>271</v>
+      </c>
+      <c r="J1" t="s">
+        <v>272</v>
+      </c>
+      <c r="K1" t="s">
+        <v>273</v>
+      </c>
+      <c r="L1" t="s">
+        <v>274</v>
+      </c>
+      <c r="M1" t="s">
+        <v>275</v>
+      </c>
+      <c r="N1" t="s">
+        <v>276</v>
+      </c>
+      <c r="O1" t="s">
+        <v>277</v>
+      </c>
+      <c r="P1" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>279</v>
+      </c>
+      <c r="R1" t="s">
+        <v>280</v>
+      </c>
+      <c r="S1" t="s">
+        <v>281</v>
+      </c>
+      <c r="T1" t="s">
+        <v>282</v>
+      </c>
+      <c r="U1" t="s">
+        <v>283</v>
+      </c>
+      <c r="V1" t="s">
+        <v>284</v>
+      </c>
+      <c r="W1" t="s">
+        <v>285</v>
+      </c>
+      <c r="X1" t="s">
+        <v>286</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>287</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>288</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>289</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>290</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>291</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1812,7 +1896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1904,7 +1988,7 @@
         <v>35.5</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1996,7 +2080,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2088,7 +2172,7 @@
         <v>41.3</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2180,7 +2264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2272,7 +2356,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2364,7 +2448,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2456,7 +2540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2548,7 +2632,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2640,7 +2724,7 @@
         <v>44.3</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2732,7 +2816,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2824,7 +2908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2916,7 +3000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -3008,7 +3092,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -3100,7 +3184,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -3192,7 +3276,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -3284,7 +3368,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -3376,7 +3460,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -3468,7 +3552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -3560,7 +3644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -3652,7 +3736,7 @@
         <v>164.7</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -3744,7 +3828,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -3836,7 +3920,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -3928,7 +4012,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -4020,7 +4104,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -4112,7 +4196,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -4204,7 +4288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -4296,7 +4380,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -4388,7 +4472,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -4480,7 +4564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -4572,7 +4656,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -4664,7 +4748,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -4756,7 +4840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -4848,7 +4932,7 @@
         <v>209.3</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -4940,7 +5024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -5032,7 +5116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -5124,7 +5208,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -5216,7 +5300,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -5308,7 +5392,7 @@
         <v>53.4</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -5400,7 +5484,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -5492,7 +5576,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -5584,7 +5668,7 @@
         <v>24.1</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -5676,7 +5760,7 @@
         <v>36.6</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -5768,7 +5852,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -5860,7 +5944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -5952,7 +6036,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -6044,7 +6128,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -6136,7 +6220,7 @@
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -6228,7 +6312,7 @@
         <v>1409.5</v>
       </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -6320,7 +6404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -6412,7 +6496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -6504,7 +6588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -6596,7 +6680,7 @@
         <v>49.1</v>
       </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -6688,7 +6772,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -6780,7 +6864,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -6872,7 +6956,7 @@
         <v>81.3</v>
       </c>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -6964,7 +7048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -7056,7 +7140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -7148,7 +7232,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -7240,7 +7324,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -7332,7 +7416,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -7424,7 +7508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -7516,7 +7600,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -7608,7 +7692,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -7700,7 +7784,7 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -7792,7 +7876,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -7884,7 +7968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -7976,7 +8060,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -8068,7 +8152,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -8160,7 +8244,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -8252,7 +8336,7 @@
         <v>97.6</v>
       </c>
     </row>
-    <row r="73" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -8344,7 +8428,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="74" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -8436,7 +8520,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -8528,7 +8612,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="76" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -8620,7 +8704,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -8712,7 +8796,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -8804,7 +8888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -8896,7 +8980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -8988,7 +9072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -9080,7 +9164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -9172,7 +9256,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="83" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -9264,7 +9348,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="84" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -9356,7 +9440,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="85" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -9448,7 +9532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -9540,7 +9624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -9632,7 +9716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -9724,7 +9808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -9816,7 +9900,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="90" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -9908,7 +9992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -10000,7 +10084,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="92" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -10092,7 +10176,7 @@
         <v>82.1</v>
       </c>
     </row>
-    <row r="93" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -10184,7 +10268,7 @@
         <v>28.8</v>
       </c>
     </row>
-    <row r="94" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -10276,7 +10360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -10368,7 +10452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -10460,7 +10544,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="97" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -10552,7 +10636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -10644,7 +10728,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="99" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -10736,7 +10820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -10828,7 +10912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -10920,7 +11004,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -11012,7 +11096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -11104,7 +11188,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="104" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -11196,7 +11280,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="105" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -11288,7 +11372,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="106" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -11380,7 +11464,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -11472,7 +11556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -11564,7 +11648,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="109" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -11656,7 +11740,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="110" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -11748,7 +11832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -11840,7 +11924,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="112" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -11932,7 +12016,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="113" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -12024,7 +12108,7 @@
         <v>1339.2</v>
       </c>
     </row>
-    <row r="114" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -12116,7 +12200,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="115" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -12208,7 +12292,7 @@
         <v>81.2</v>
       </c>
     </row>
-    <row r="116" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -12300,7 +12384,7 @@
         <v>38.299999999999997</v>
       </c>
     </row>
-    <row r="117" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -12392,7 +12476,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="118" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -12484,7 +12568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -12576,7 +12660,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="120" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -12668,7 +12752,7 @@
         <v>59.4</v>
       </c>
     </row>
-    <row r="121" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -12760,7 +12844,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="122" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -12852,7 +12936,7 @@
         <v>127.5</v>
       </c>
     </row>
-    <row r="123" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -12944,7 +13028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -13036,7 +13120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -13128,7 +13212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -13220,7 +13304,7 @@
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="127" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -13312,7 +13396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -13404,7 +13488,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="129" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -13496,7 +13580,7 @@
         <v>49.7</v>
       </c>
     </row>
-    <row r="130" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -13588,7 +13672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -13680,7 +13764,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="132" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -13772,7 +13856,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="133" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -13864,7 +13948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="134" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -13956,7 +14040,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="135" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -14048,7 +14132,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="136" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -14140,7 +14224,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="137" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -14232,7 +14316,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="138" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -14324,7 +14408,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="139" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -14416,7 +14500,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="140" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -14508,7 +14592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -14600,7 +14684,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="142" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -14692,7 +14776,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="143" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -14784,7 +14868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -14876,7 +14960,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="145" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -14968,7 +15052,7 @@
         <v>25.6</v>
       </c>
     </row>
-    <row r="146" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -15060,7 +15144,7 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="147" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -15152,7 +15236,7 @@
         <v>31.6</v>
       </c>
     </row>
-    <row r="148" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -15244,7 +15328,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="149" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -15336,7 +15420,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="150" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -15428,7 +15512,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="151" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -15520,7 +15604,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="152" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>151</v>
       </c>
@@ -15612,7 +15696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -15704,7 +15788,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="154" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -15796,7 +15880,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="155" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -15888,7 +15972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -15980,7 +16064,7 @@
         <v>129.19999999999999</v>
       </c>
     </row>
-    <row r="157" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -16072,7 +16156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>157</v>
       </c>
@@ -16164,7 +16248,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="159" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>158</v>
       </c>
@@ -16256,7 +16340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -16348,7 +16432,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="161" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>160</v>
       </c>
@@ -16440,7 +16524,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="162" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -16532,7 +16616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -16624,7 +16708,7 @@
         <v>35.700000000000003</v>
       </c>
     </row>
-    <row r="164" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -16716,7 +16800,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="165" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -16808,7 +16892,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="166" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -16900,7 +16984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -16992,7 +17076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -17084,7 +17168,7 @@
         <v>29.3</v>
       </c>
     </row>
-    <row r="169" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -17176,7 +17260,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -17268,7 +17352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -17360,7 +17444,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="172" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -17452,7 +17536,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="173" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -17544,7 +17628,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="174" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -17636,7 +17720,7 @@
         <v>190.9</v>
       </c>
     </row>
-    <row r="175" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -17728,7 +17812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -17820,7 +17904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>176</v>
       </c>
@@ -17912,7 +17996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>177</v>
       </c>
@@ -18004,7 +18088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>178</v>
       </c>
@@ -18096,7 +18180,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="180" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>179</v>
       </c>
@@ -18188,7 +18272,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="181" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>180</v>
       </c>
@@ -18280,7 +18364,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="182" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>181</v>
       </c>
@@ -18372,7 +18456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>182</v>
       </c>
@@ -18464,7 +18548,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="184" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>183</v>
       </c>
@@ -18556,7 +18640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>184</v>
       </c>
@@ -18648,7 +18732,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="186" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>185</v>
       </c>
@@ -18740,7 +18824,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="187" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>186</v>
       </c>
@@ -18832,7 +18916,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="188" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>187</v>
       </c>
@@ -18924,7 +19008,7 @@
         <v>32.200000000000003</v>
       </c>
     </row>
-    <row r="189" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>188</v>
       </c>
@@ -19016,7 +19100,7 @@
         <v>104.9</v>
       </c>
     </row>
-    <row r="190" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>189</v>
       </c>
@@ -19108,7 +19192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>190</v>
       </c>
@@ -19200,7 +19284,7 @@
         <v>38.200000000000003</v>
       </c>
     </row>
-    <row r="192" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>191</v>
       </c>
@@ -19292,7 +19376,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="193" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -19384,7 +19468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>193</v>
       </c>
@@ -19476,7 +19560,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="195" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>194</v>
       </c>
@@ -19568,7 +19652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>195</v>
       </c>
@@ -19660,7 +19744,7 @@
         <v>19.7</v>
       </c>
     </row>
-    <row r="197" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>196</v>
       </c>
@@ -19752,7 +19836,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="198" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>197</v>
       </c>
@@ -19844,7 +19928,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="199" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>198</v>
       </c>
@@ -19936,7 +20020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -20028,7 +20112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>200</v>
       </c>
@@ -20120,7 +20204,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="202" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -20212,7 +20296,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="203" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>202</v>
       </c>
@@ -20304,7 +20388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>203</v>
       </c>
@@ -20396,7 +20480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>204</v>
       </c>
@@ -20488,7 +20572,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="206" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -20580,7 +20664,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="207" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -20672,7 +20756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -20764,7 +20848,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="209" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -20856,7 +20940,7 @@
         <v>32.9</v>
       </c>
     </row>
-    <row r="210" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -20948,7 +21032,7 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="211" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -21040,7 +21124,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="212" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>211</v>
       </c>
@@ -21132,7 +21216,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="213" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>212</v>
       </c>
@@ -21224,7 +21308,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="214" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -21316,7 +21400,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="215" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>214</v>
       </c>
@@ -21408,7 +21492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -21500,7 +21584,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="217" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>216</v>
       </c>
@@ -21592,7 +21676,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="218" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -21684,7 +21768,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="219" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -21776,7 +21860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>219</v>
       </c>
@@ -21868,7 +21952,7 @@
         <v>56.7</v>
       </c>
     </row>
-    <row r="221" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -21960,7 +22044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>221</v>
       </c>
@@ -22052,7 +22136,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="223" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>222</v>
       </c>
@@ -22144,7 +22228,7 @@
         <v>46.4</v>
       </c>
     </row>
-    <row r="224" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>223</v>
       </c>
@@ -22236,7 +22320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>224</v>
       </c>
@@ -22328,7 +22412,7 @@
         <v>20.9</v>
       </c>
     </row>
-    <row r="226" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>225</v>
       </c>
@@ -22420,7 +22504,7 @@
         <v>40.5</v>
       </c>
     </row>
-    <row r="227" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>226</v>
       </c>
@@ -22512,7 +22596,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="228" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>227</v>
       </c>
@@ -22604,7 +22688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>228</v>
       </c>
@@ -22696,7 +22780,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="230" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>229</v>
       </c>
@@ -22788,7 +22872,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="231" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>230</v>
       </c>
@@ -22880,7 +22964,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="232" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>231</v>
       </c>
@@ -22972,7 +23056,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="233" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>232</v>
       </c>
@@ -23064,7 +23148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>233</v>
       </c>
@@ -23156,7 +23240,7 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="235" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>234</v>
       </c>
@@ -23248,7 +23332,7 @@
         <v>57.3</v>
       </c>
     </row>
-    <row r="236" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>235</v>
       </c>
@@ -23340,7 +23424,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="237" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>236</v>
       </c>
@@ -23432,7 +23516,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="238" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>237</v>
       </c>
@@ -23524,7 +23608,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="239" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>238</v>
       </c>
@@ -23616,7 +23700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>239</v>
       </c>
@@ -23708,7 +23792,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="241" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>240</v>
       </c>
@@ -23800,7 +23884,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="242" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>241</v>
       </c>
@@ -23892,7 +23976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>242</v>
       </c>
@@ -23984,7 +24068,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="244" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>243</v>
       </c>
@@ -24076,7 +24160,7 @@
         <v>80.7</v>
       </c>
     </row>
-    <row r="245" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>244</v>
       </c>
@@ -24168,7 +24252,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="246" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>245</v>
       </c>
@@ -24260,7 +24344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>246</v>
       </c>
@@ -24352,7 +24436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>247</v>
       </c>
@@ -24444,7 +24528,7 @@
         <v>42.9</v>
       </c>
     </row>
-    <row r="249" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>248</v>
       </c>
@@ -24536,7 +24620,7 @@
         <v>44.2</v>
       </c>
     </row>
-    <row r="250" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -24628,7 +24712,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="251" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>250</v>
       </c>
@@ -24720,7 +24804,7 @@
         <v>66.2</v>
       </c>
     </row>
-    <row r="252" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>251</v>
       </c>
@@ -24812,7 +24896,7 @@
         <v>324.5</v>
       </c>
     </row>
-    <row r="253" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>252</v>
       </c>
@@ -24904,7 +24988,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="254" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>253</v>
       </c>
@@ -24996,7 +25080,7 @@
         <v>31.9</v>
       </c>
     </row>
-    <row r="255" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>254</v>
       </c>
@@ -25088,7 +25172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -25180,7 +25264,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="257" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>256</v>
       </c>
@@ -25272,7 +25356,7 @@
         <v>95.5</v>
       </c>
     </row>
-    <row r="258" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>257</v>
       </c>
@@ -25364,7 +25448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>258</v>
       </c>
@@ -25456,7 +25540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>259</v>
       </c>
@@ -25548,7 +25632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>260</v>
       </c>
@@ -25640,7 +25724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>261</v>
       </c>
@@ -25732,7 +25816,7 @@
         <v>28.3</v>
       </c>
     </row>
-    <row r="263" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>262</v>
       </c>
@@ -25824,7 +25908,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="264" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>263</v>
       </c>
@@ -25916,7 +26000,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="265" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>264</v>
       </c>

</xml_diff>